<commit_message>
Family planning update using fraction population targeted
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Master/MasterTemplate.xlsx
+++ b/input_spreadsheets/Master/MasterTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="-21140" windowWidth="28460" windowHeight="20120" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34840" yWindow="-21140" windowWidth="28460" windowHeight="20120" tabRatio="500" firstSheet="14" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,10 @@
     <sheet name="Program dependencies" sheetId="40" r:id="rId24"/>
     <sheet name="Program risk areas" sheetId="36" r:id="rId25"/>
     <sheet name="Population risk areas" sheetId="43" r:id="rId26"/>
-    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId27"/>
-    <sheet name="Reference programs" sheetId="48" r:id="rId28"/>
-    <sheet name="Programs to include" sheetId="44" r:id="rId29"/>
+    <sheet name="Programs annual scale-up" sheetId="51" r:id="rId27"/>
+    <sheet name="Programs cost and coverage" sheetId="20" r:id="rId28"/>
+    <sheet name="Reference programs" sheetId="48" r:id="rId29"/>
+    <sheet name="Programs to include" sheetId="44" r:id="rId30"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1749,6 +1750,49 @@
 </comments>
 </file>
 
+<file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{45B4E5D3-C5DC-6B43-822A-DF0A04E4F811}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Constrains the coverage % scale-up from baseline</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
@@ -2448,7 +2492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="270">
   <si>
     <t>year</t>
   </si>
@@ -3256,6 +3300,9 @@
   <si>
     <t>Calculated in model</t>
   </si>
+  <si>
+    <t>Maximum annual scale-up</t>
+  </si>
 </sst>
 </file>
 
@@ -3267,7 +3314,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3392,6 +3439,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3402,6 +3455,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4556,11 +4616,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -6707,7 +6767,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7501,7 +7561,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="127" t="s">
+      <c r="A22" s="126" t="s">
         <v>218</v>
       </c>
       <c r="B22" t="s">
@@ -7575,7 +7635,7 @@
       <c r="A2" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="127" t="s">
         <v>73</v>
       </c>
       <c r="C2" t="s">
@@ -7598,7 +7658,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="125"/>
+      <c r="B3" s="127"/>
       <c r="C3" t="s">
         <v>154</v>
       </c>
@@ -7620,7 +7680,7 @@
       <c r="J3" s="51"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="125"/>
+      <c r="B4" s="127"/>
       <c r="C4" t="s">
         <v>164</v>
       </c>
@@ -7647,7 +7707,7 @@
       <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -7670,7 +7730,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" t="s">
         <v>154</v>
       </c>
@@ -7691,7 +7751,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" t="s">
         <v>164</v>
       </c>
@@ -7717,7 +7777,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="125" t="s">
+      <c r="B8" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -7740,7 +7800,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" t="s">
         <v>154</v>
       </c>
@@ -7761,7 +7821,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="125"/>
+      <c r="B10" s="127"/>
       <c r="C10" t="s">
         <v>164</v>
       </c>
@@ -7786,7 +7846,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -7809,7 +7869,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="125"/>
+      <c r="B12" s="127"/>
       <c r="C12" t="s">
         <v>154</v>
       </c>
@@ -7830,7 +7890,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" t="s">
         <v>164</v>
       </c>
@@ -7854,7 +7914,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="125" t="s">
+      <c r="B14" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -7877,7 +7937,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="125"/>
+      <c r="B15" s="127"/>
       <c r="C15" t="s">
         <v>154</v>
       </c>
@@ -7898,7 +7958,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="125"/>
+      <c r="B16" s="127"/>
       <c r="C16" t="s">
         <v>164</v>
       </c>
@@ -7954,7 +8014,7 @@
       <c r="A19" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="127" t="s">
         <v>73</v>
       </c>
       <c r="C19" t="s">
@@ -7977,7 +8037,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="125"/>
+      <c r="B20" s="127"/>
       <c r="C20" t="s">
         <v>154</v>
       </c>
@@ -7998,7 +8058,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="125"/>
+      <c r="B21" s="127"/>
       <c r="C21" t="s">
         <v>164</v>
       </c>
@@ -8024,7 +8084,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="125" t="s">
+      <c r="B22" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -8047,7 +8107,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="125"/>
+      <c r="B23" s="127"/>
       <c r="C23" t="s">
         <v>154</v>
       </c>
@@ -8068,7 +8128,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="125"/>
+      <c r="B24" s="127"/>
       <c r="C24" t="s">
         <v>164</v>
       </c>
@@ -8094,7 +8154,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="125" t="s">
+      <c r="B25" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -8117,7 +8177,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="125"/>
+      <c r="B26" s="127"/>
       <c r="C26" t="s">
         <v>154</v>
       </c>
@@ -8138,7 +8198,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="125"/>
+      <c r="B27" s="127"/>
       <c r="C27" t="s">
         <v>164</v>
       </c>
@@ -8164,7 +8224,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -8187,7 +8247,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="125"/>
+      <c r="B29" s="127"/>
       <c r="C29" t="s">
         <v>154</v>
       </c>
@@ -8208,7 +8268,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="125"/>
+      <c r="B30" s="127"/>
       <c r="C30" t="s">
         <v>164</v>
       </c>
@@ -8234,7 +8294,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="125" t="s">
+      <c r="B31" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -8257,7 +8317,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="125"/>
+      <c r="B32" s="127"/>
       <c r="C32" t="s">
         <v>154</v>
       </c>
@@ -8278,7 +8338,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B33" s="125"/>
+      <c r="B33" s="127"/>
       <c r="C33" t="s">
         <v>164</v>
       </c>
@@ -8330,7 +8390,7 @@
       <c r="A36" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B36" s="125" t="s">
+      <c r="B36" s="127" t="s">
         <v>73</v>
       </c>
       <c r="C36" t="s">
@@ -8353,7 +8413,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B37" s="125"/>
+      <c r="B37" s="127"/>
       <c r="C37" t="s">
         <v>154</v>
       </c>
@@ -8374,7 +8434,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B38" s="125"/>
+      <c r="B38" s="127"/>
       <c r="C38" t="s">
         <v>164</v>
       </c>
@@ -8395,7 +8455,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B39" s="125" t="s">
+      <c r="B39" s="127" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -8418,7 +8478,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B40" s="125"/>
+      <c r="B40" s="127"/>
       <c r="C40" t="s">
         <v>154</v>
       </c>
@@ -8439,7 +8499,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B41" s="125"/>
+      <c r="B41" s="127"/>
       <c r="C41" t="s">
         <v>164</v>
       </c>
@@ -8460,7 +8520,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B42" s="125" t="s">
+      <c r="B42" s="127" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -8483,7 +8543,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B43" s="125"/>
+      <c r="B43" s="127"/>
       <c r="C43" t="s">
         <v>154</v>
       </c>
@@ -8504,7 +8564,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B44" s="125"/>
+      <c r="B44" s="127"/>
       <c r="C44" t="s">
         <v>164</v>
       </c>
@@ -8525,7 +8585,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B45" s="125" t="s">
+      <c r="B45" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -8548,7 +8608,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B46" s="125"/>
+      <c r="B46" s="127"/>
       <c r="C46" t="s">
         <v>154</v>
       </c>
@@ -8569,7 +8629,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B47" s="125"/>
+      <c r="B47" s="127"/>
       <c r="C47" t="s">
         <v>164</v>
       </c>
@@ -8590,7 +8650,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B48" s="125" t="s">
+      <c r="B48" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -8613,7 +8673,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="125"/>
+      <c r="B49" s="127"/>
       <c r="C49" t="s">
         <v>154</v>
       </c>
@@ -8634,7 +8694,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="125"/>
+      <c r="B50" s="127"/>
       <c r="C50" t="s">
         <v>164</v>
       </c>
@@ -8679,6 +8739,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -8689,11 +8754,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12255,7 +12315,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13363,8 +13423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14962,16 +15022,20 @@
         <v>0</v>
       </c>
       <c r="L36" s="115">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.1</v>
       </c>
       <c r="M36" s="115">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.1</v>
       </c>
       <c r="N36" s="115">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.1</v>
       </c>
       <c r="O36" s="115">
-        <v>1</v>
+        <f>'Programs cost and coverage'!$B6 + 'Baseline year demographics'!$C12</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15752,8 +15816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18175,7 +18239,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19486,11 +19550,516 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC6050C-0865-7046-B5F3-F185B3ED8E81}">
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="str">
+        <f>'Programs to include'!A2</f>
+        <v>Balanced energy-protein supplementation</v>
+      </c>
+      <c r="B2" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>'Programs to include'!A3</f>
+        <v>Birth age program</v>
+      </c>
+      <c r="B3" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f>'Programs to include'!A4</f>
+        <v>Calcium supplementation</v>
+      </c>
+      <c r="B4" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
+        <f>'Programs to include'!A5</f>
+        <v>Cash transfers</v>
+      </c>
+      <c r="B5" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>'Programs to include'!A6</f>
+        <v>Family Planning</v>
+      </c>
+      <c r="B6" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>'Programs to include'!A7</f>
+        <v>IFA fortification of maize</v>
+      </c>
+      <c r="B7" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
+        <f>'Programs to include'!A8</f>
+        <v>IFA fortification of rice</v>
+      </c>
+      <c r="B8" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
+        <f>'Programs to include'!A9</f>
+        <v>IFA fortification of wheat flour</v>
+      </c>
+      <c r="B9" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="str">
+        <f>'Programs to include'!A10</f>
+        <v>IFAS not poor: community</v>
+      </c>
+      <c r="B10" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
+        <f>'Programs to include'!A11</f>
+        <v>IFAS not poor: community (malaria area)</v>
+      </c>
+      <c r="B11" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
+        <f>'Programs to include'!A12</f>
+        <v>IFAS not poor: hospital</v>
+      </c>
+      <c r="B12" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="str">
+        <f>'Programs to include'!A13</f>
+        <v>IFAS not poor: hospital (malaria area)</v>
+      </c>
+      <c r="B13" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="str">
+        <f>'Programs to include'!A14</f>
+        <v>IFAS not poor: retailer</v>
+      </c>
+      <c r="B14" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="str">
+        <f>'Programs to include'!A15</f>
+        <v>IFAS not poor: retailer (malaria area)</v>
+      </c>
+      <c r="B15" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="str">
+        <f>'Programs to include'!A16</f>
+        <v>IFAS not poor: school</v>
+      </c>
+      <c r="B16" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f>'Programs to include'!A17</f>
+        <v>IFAS not poor: school (malaria area)</v>
+      </c>
+      <c r="B17" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f>'Programs to include'!A18</f>
+        <v>IFAS poor: community</v>
+      </c>
+      <c r="B18" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="str">
+        <f>'Programs to include'!A19</f>
+        <v>IFAS poor: community (malaria area)</v>
+      </c>
+      <c r="B19" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="str">
+        <f>'Programs to include'!A20</f>
+        <v>IFAS poor: hospital</v>
+      </c>
+      <c r="B20" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="str">
+        <f>'Programs to include'!A21</f>
+        <v>IFAS poor: hospital (malaria area)</v>
+      </c>
+      <c r="B21" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="str">
+        <f>'Programs to include'!A22</f>
+        <v>IFAS poor: school</v>
+      </c>
+      <c r="B22" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="str">
+        <f>'Programs to include'!A23</f>
+        <v>IFAS poor: school (malaria area)</v>
+      </c>
+      <c r="B23" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f>'Programs to include'!A24</f>
+        <v>IPTp</v>
+      </c>
+      <c r="B24" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f>'Programs to include'!A25</f>
+        <v>Iron and folic acid supplementation for pregnant women</v>
+      </c>
+      <c r="B25" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f>'Programs to include'!A26</f>
+        <v>Iron and folic acid supplementation for pregnant women (malaria area)</v>
+      </c>
+      <c r="B26" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f>'Programs to include'!A27</f>
+        <v>Iron and iodine fortification of salt</v>
+      </c>
+      <c r="B27" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f>'Programs to include'!A28</f>
+        <v>Iron fortification of maize</v>
+      </c>
+      <c r="B28" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="str">
+        <f>'Programs to include'!A29</f>
+        <v>Iron fortification of rice</v>
+      </c>
+      <c r="B29" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="str">
+        <f>'Programs to include'!A30</f>
+        <v>Iron fortification of wheat flour</v>
+      </c>
+      <c r="B30" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="str">
+        <f>'Programs to include'!A31</f>
+        <v>Long-lasting insecticide-treated bednets</v>
+      </c>
+      <c r="B31" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="str">
+        <f>'Programs to include'!A32</f>
+        <v>Mg for eclampsia</v>
+      </c>
+      <c r="B32" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="str">
+        <f>'Programs to include'!A33</f>
+        <v>Mg for pre-eclampsia</v>
+      </c>
+      <c r="B33" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="str">
+        <f>'Programs to include'!A34</f>
+        <v>Multiple micronutrient supplementation</v>
+      </c>
+      <c r="B34" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="str">
+        <f>'Programs to include'!A35</f>
+        <v>Multiple micronutrient supplementation (malaria area)</v>
+      </c>
+      <c r="B35" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="str">
+        <f>'Programs to include'!A36</f>
+        <v>Oral rehydration salts</v>
+      </c>
+      <c r="B36" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="str">
+        <f>'Programs to include'!A37</f>
+        <v>Public provision of complementary foods</v>
+      </c>
+      <c r="B37" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="str">
+        <f>'Programs to include'!A38</f>
+        <v>Public provision of complementary foods with iron</v>
+      </c>
+      <c r="B38" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="str">
+        <f>'Programs to include'!A39</f>
+        <v>Public provision of complementary foods with iron (malaria area)</v>
+      </c>
+      <c r="B39" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="str">
+        <f>'Programs to include'!A40</f>
+        <v>Sprinkles</v>
+      </c>
+      <c r="B40" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="str">
+        <f>'Programs to include'!A41</f>
+        <v>Sprinkles (malaria area)</v>
+      </c>
+      <c r="B41" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="str">
+        <f>'Programs to include'!A42</f>
+        <v>Treatment of MAM</v>
+      </c>
+      <c r="B42" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="str">
+        <f>'Programs to include'!A43</f>
+        <v>Treatment of SAM</v>
+      </c>
+      <c r="B43" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="str">
+        <f>'Programs to include'!A44</f>
+        <v>Vitamin A supplementation</v>
+      </c>
+      <c r="B44" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="str">
+        <f>'Programs to include'!A45</f>
+        <v>WASH: Handwashing</v>
+      </c>
+      <c r="B45" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="str">
+        <f>'Programs to include'!A46</f>
+        <v>WASH: Hygenic disposal</v>
+      </c>
+      <c r="B46" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="str">
+        <f>'Programs to include'!A47</f>
+        <v>WASH: Improved sanitation</v>
+      </c>
+      <c r="B47" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="str">
+        <f>'Programs to include'!A48</f>
+        <v>WASH: Improved water source</v>
+      </c>
+      <c r="B48" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="str">
+        <f>'Programs to include'!A49</f>
+        <v>WASH: Piped water</v>
+      </c>
+      <c r="B49" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="str">
+        <f>'Programs to include'!A50</f>
+        <v>Zinc for treatment + ORS</v>
+      </c>
+      <c r="B50" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="str">
+        <f>'Programs to include'!A51</f>
+        <v>Zinc supplementation</v>
+      </c>
+      <c r="B51" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="str">
+        <f>'Programs to include'!A52</f>
+        <v>IYCF 1</v>
+      </c>
+      <c r="B52" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="str">
+        <f>'Programs to include'!A53</f>
+        <v>IYCF 2</v>
+      </c>
+      <c r="B53" s="86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="str">
+        <f>'Programs to include'!A54</f>
+        <v>IYCF 3</v>
+      </c>
+      <c r="B54" s="86">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20340,12 +20909,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8166B-8704-DF4E-9AA8-4565893AE0CB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20398,453 +20967,6 @@
       <c r="A9" t="s">
         <v>257</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:B54"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="122" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="124" t="s">
-        <v>266</v>
-      </c>
-      <c r="B3" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="B4" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="122" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B8" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="122" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="122" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="122" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="122" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="122" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="122" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="122" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="122" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="122" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="122" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="122" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="122" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="122" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="122" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="122" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="116" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="123"/>
-    </row>
-    <row r="29" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="116" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="123"/>
-    </row>
-    <row r="30" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="123"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B32" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B33" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="122" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="122" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="122" t="s">
-        <v>261</v>
-      </c>
-      <c r="B36" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B39" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B42" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="122" t="s">
-        <v>260</v>
-      </c>
-      <c r="B45" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="122" t="s">
-        <v>259</v>
-      </c>
-      <c r="B46" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="122" t="s">
-        <v>258</v>
-      </c>
-      <c r="B47" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="122" t="s">
-        <v>256</v>
-      </c>
-      <c r="B48" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="122" t="s">
-        <v>257</v>
-      </c>
-      <c r="B49" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="122" t="s">
-        <v>262</v>
-      </c>
-      <c r="B50" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="126" t="s">
-        <v>161</v>
-      </c>
-      <c r="B52" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="126" t="s">
-        <v>162</v>
-      </c>
-      <c r="B53" s="122" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="126" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" s="122"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21773,11 +21895,458 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="122" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="124" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="122" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="122" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="122" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="122" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="122" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="122" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="122" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="122" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="122" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="122" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="116" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="123"/>
+    </row>
+    <row r="29" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="116" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="123"/>
+    </row>
+    <row r="30" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="123"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B32" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B33" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="122" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="122" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="122" t="s">
+        <v>261</v>
+      </c>
+      <c r="B36" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" s="122" t="s">
+        <v>260</v>
+      </c>
+      <c r="B45" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" s="122" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" s="122" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" s="122" t="s">
+        <v>256</v>
+      </c>
+      <c r="B48" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" s="122" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" s="122" t="s">
+        <v>262</v>
+      </c>
+      <c r="B50" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" s="125" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="125" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="122" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="125" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="122"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>

</xml_diff>